<commit_message>
updating after a while
</commit_message>
<xml_diff>
--- a/application/example.xlsx
+++ b/application/example.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,25 +700,29 @@
           <t>BTEX</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.108</t>
         </is>
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.146</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.135</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.145</t>
         </is>
       </c>
       <c r="G14" s="1" t="n"/>
@@ -730,7 +734,11 @@
           <t>THM</t>
         </is>
       </c>
-      <c r="B15" s="1" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
           <t>ND</t>
@@ -760,7 +768,11 @@
           <t>THM</t>
         </is>
       </c>
-      <c r="B16" s="1" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
           <t>ND</t>
@@ -790,25 +802,29 @@
           <t>Turb</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n"/>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.0045</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.0047</t>
         </is>
       </c>
       <c r="E17" s="10" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.0041</t>
         </is>
       </c>
       <c r="F17" s="10" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.0039</t>
         </is>
       </c>
       <c r="G17" s="9" t="n"/>
@@ -916,10 +932,14 @@
           <t>BTEX</t>
         </is>
       </c>
-      <c r="B24" s="1" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.112</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
@@ -946,7 +966,11 @@
           <t>THM</t>
         </is>
       </c>
-      <c r="B25" s="1" t="n"/>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
           <t>ND</t>
@@ -976,7 +1000,11 @@
           <t>THM</t>
         </is>
       </c>
-      <c r="B26" s="1" t="n"/>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
           <t>ND</t>
@@ -1006,10 +1034,14 @@
           <t>Turb</t>
         </is>
       </c>
-      <c r="B27" s="9" t="n"/>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
       <c r="C27" s="10" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>0.0044</t>
         </is>
       </c>
       <c r="D27" s="10" t="inlineStr">
@@ -1043,7 +1075,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>SD   = standard devition;       REF VALUE = primary or secondary reference material</t>
+          <t>SD    = standard devition;       REF VALUE = primary or secondary reference material</t>
         </is>
       </c>
       <c r="B29" s="1" t="n"/>
@@ -1071,7 +1103,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>So   = standard deviation at zero analyte concentration; method detection limit is generally</t>
+          <t>So     = standard deviation at zero analyte concentration; method detection limit is generally</t>
         </is>
       </c>
       <c r="B31" s="1" t="n"/>
@@ -1099,7 +1131,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>ND   = none is detcted;         n/a = not applicable</t>
+          <t>ND   = none is detcted;          n/a = not applicable</t>
         </is>
       </c>
       <c r="B33" s="1" t="n"/>
@@ -1110,6 +1142,7 @@
       <c r="G33" s="1" t="n"/>
       <c r="H33" s="1" t="n"/>
     </row>
+    <row r="50"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A9:H10"/>

</xml_diff>